<commit_message>
Updated values for some dwc fields
</commit_message>
<xml_diff>
--- a/DwC/HABsDwC.xlsx
+++ b/DwC/HABsDwC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianbr\Documents\EDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianbr\Documents\EDI\sccoos_git\HABsDataPublish\DwC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F91D292-3DD5-4E80-8743-CF31942E034A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F79F2D-77BE-4054-87D6-A1341F776C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4125" yWindow="3465" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="125">
   <si>
     <t>measurementType</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>http://vocab.nerc.ac.uk/collection/P25/current/SLCA/; https://www.bco-dmo.org/parameter/1209</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P09/current/PSAL/</t>
   </si>
 </sst>
 </file>
@@ -809,7 +812,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -994,6 +997,9 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1499,7 +1505,7 @@
   <customSheetViews>
     <customSheetView guid="{FC104643-3A9D-4181-8925-6DE3D4A25C75}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2" xr:uid="{66A4033A-4763-4CFD-AD71-A35532B714AB}"/>
+      <autoFilter ref="A2" xr:uid="{C3D4630C-DD9E-45E5-869B-CBA9456395B2}"/>
     </customSheetView>
   </customSheetViews>
   <hyperlinks>

</xml_diff>